<commit_message>
DS, HT and MA done
</commit_message>
<xml_diff>
--- a/_alcoholism_patterns/_data/Data_checked/verified_alcoholism_survey.xlsx
+++ b/_alcoholism_patterns/_data/Data_checked/verified_alcoholism_survey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="verified_alcoholism_survey" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3975" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3944" uniqueCount="54">
   <si>
     <t>Consecutivo</t>
   </si>
@@ -1003,7 +1003,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O327"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -16398,7 +16398,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O327"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A305" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:O327"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -17320,8 +17322,8 @@
       <c r="E20">
         <v>0</v>
       </c>
-      <c r="F20" t="s">
-        <v>17</v>
+      <c r="F20">
+        <v>9999</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -17496,14 +17498,14 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" t="s">
-        <v>17</v>
+      <c r="B24">
+        <v>9999</v>
+      </c>
+      <c r="C24" s="3">
+        <v>9999</v>
+      </c>
+      <c r="D24">
+        <v>9999</v>
       </c>
       <c r="E24">
         <v>1</v>
@@ -18107,8 +18109,8 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" t="s">
-        <v>17</v>
+      <c r="B37">
+        <v>9999</v>
       </c>
       <c r="C37" s="3">
         <v>18</v>
@@ -18204,8 +18206,8 @@
       <c r="B39">
         <v>2</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>17</v>
+      <c r="C39" s="3">
+        <v>9999</v>
       </c>
       <c r="D39">
         <v>11</v>
@@ -18495,17 +18497,17 @@
       <c r="E45">
         <v>0</v>
       </c>
-      <c r="F45" t="s">
-        <v>17</v>
+      <c r="F45">
+        <v>9999</v>
       </c>
       <c r="G45">
         <v>0</v>
       </c>
-      <c r="H45" t="s">
-        <v>17</v>
-      </c>
-      <c r="I45" t="s">
-        <v>17</v>
+      <c r="H45">
+        <v>9999</v>
+      </c>
+      <c r="I45">
+        <v>9999</v>
       </c>
       <c r="J45">
         <v>0</v>
@@ -18683,8 +18685,8 @@
       <c r="E49">
         <v>0</v>
       </c>
-      <c r="F49" t="s">
-        <v>17</v>
+      <c r="F49">
+        <v>9999</v>
       </c>
       <c r="G49">
         <v>0</v>
@@ -19344,8 +19346,8 @@
       <c r="F63">
         <v>3</v>
       </c>
-      <c r="G63" t="s">
-        <v>17</v>
+      <c r="G63">
+        <v>9999</v>
       </c>
       <c r="H63">
         <v>1</v>
@@ -19717,8 +19719,8 @@
       <c r="E71">
         <v>0</v>
       </c>
-      <c r="F71" t="s">
-        <v>17</v>
+      <c r="F71">
+        <v>9999</v>
       </c>
       <c r="G71">
         <v>0</v>
@@ -20093,8 +20095,8 @@
       <c r="E79">
         <v>0</v>
       </c>
-      <c r="F79" t="s">
-        <v>17</v>
+      <c r="F79">
+        <v>9999</v>
       </c>
       <c r="G79">
         <v>0</v>
@@ -20672,8 +20674,8 @@
       <c r="J91">
         <v>0</v>
       </c>
-      <c r="K91" t="s">
-        <v>17</v>
+      <c r="K91">
+        <v>9999</v>
       </c>
       <c r="L91">
         <v>0</v>
@@ -20739,8 +20741,8 @@
       <c r="A93">
         <v>92</v>
       </c>
-      <c r="B93" t="s">
-        <v>17</v>
+      <c r="B93">
+        <v>9999</v>
       </c>
       <c r="C93" s="3">
         <v>19</v>
@@ -22290,8 +22292,8 @@
       <c r="A126">
         <v>125</v>
       </c>
-      <c r="B126" t="s">
-        <v>17</v>
+      <c r="B126">
+        <v>9999</v>
       </c>
       <c r="C126" s="3">
         <v>18</v>
@@ -22666,8 +22668,8 @@
       <c r="A134">
         <v>133</v>
       </c>
-      <c r="B134" t="s">
-        <v>17</v>
+      <c r="B134">
+        <v>9999</v>
       </c>
       <c r="C134" s="3">
         <v>18</v>
@@ -23101,8 +23103,8 @@
       <c r="E143">
         <v>0</v>
       </c>
-      <c r="F143" t="s">
-        <v>17</v>
+      <c r="F143">
+        <v>9999</v>
       </c>
       <c r="G143">
         <v>0</v>
@@ -23935,8 +23937,8 @@
       <c r="A161">
         <v>160</v>
       </c>
-      <c r="B161" t="s">
-        <v>17</v>
+      <c r="B161">
+        <v>9999</v>
       </c>
       <c r="C161" s="3">
         <v>17</v>
@@ -25357,8 +25359,8 @@
       <c r="E191">
         <v>0</v>
       </c>
-      <c r="F191" t="s">
-        <v>17</v>
+      <c r="F191">
+        <v>9999</v>
       </c>
       <c r="G191">
         <v>0</v>
@@ -25381,8 +25383,8 @@
       <c r="M191">
         <v>0</v>
       </c>
-      <c r="N191" t="s">
-        <v>17</v>
+      <c r="N191">
+        <v>9999</v>
       </c>
       <c r="O191" s="2">
         <v>0</v>
@@ -26720,8 +26722,8 @@
       <c r="E220">
         <v>0</v>
       </c>
-      <c r="F220" t="s">
-        <v>17</v>
+      <c r="F220">
+        <v>9999</v>
       </c>
       <c r="G220">
         <v>0</v>
@@ -27055,8 +27057,8 @@
       <c r="G227">
         <v>1</v>
       </c>
-      <c r="H227" t="s">
-        <v>17</v>
+      <c r="H227">
+        <v>9999</v>
       </c>
       <c r="I227">
         <v>0</v>
@@ -27308,8 +27310,8 @@
       <c r="M232">
         <v>0</v>
       </c>
-      <c r="N232" t="s">
-        <v>17</v>
+      <c r="N232">
+        <v>9999</v>
       </c>
       <c r="O232" s="2">
         <v>5</v>
@@ -27836,8 +27838,8 @@
       <c r="A244">
         <v>243</v>
       </c>
-      <c r="B244" t="s">
-        <v>17</v>
+      <c r="B244">
+        <v>9999</v>
       </c>
       <c r="C244" s="3">
         <v>16</v>
@@ -27883,8 +27885,8 @@
       <c r="A245">
         <v>244</v>
       </c>
-      <c r="B245" t="s">
-        <v>17</v>
+      <c r="B245">
+        <v>9999</v>
       </c>
       <c r="C245" s="3">
         <v>17</v>
@@ -29058,8 +29060,8 @@
       <c r="A270">
         <v>269</v>
       </c>
-      <c r="B270" t="s">
-        <v>17</v>
+      <c r="B270">
+        <v>9999</v>
       </c>
       <c r="C270" s="3">
         <v>17</v>
@@ -30186,8 +30188,8 @@
       <c r="A294">
         <v>293</v>
       </c>
-      <c r="B294" t="s">
-        <v>17</v>
+      <c r="B294">
+        <v>9999</v>
       </c>
       <c r="C294" s="3">
         <v>18</v>
@@ -30750,8 +30752,8 @@
       <c r="A306">
         <v>305</v>
       </c>
-      <c r="B306" t="s">
-        <v>17</v>
+      <c r="B306">
+        <v>9999</v>
       </c>
       <c r="C306" s="3">
         <v>17</v>
@@ -31032,8 +31034,8 @@
       <c r="A312">
         <v>311</v>
       </c>
-      <c r="B312" t="s">
-        <v>17</v>
+      <c r="B312">
+        <v>9999</v>
       </c>
       <c r="C312" s="3">
         <v>16</v>
@@ -31549,8 +31551,8 @@
       <c r="A323">
         <v>322</v>
       </c>
-      <c r="B323" t="s">
-        <v>17</v>
+      <c r="B323">
+        <v>9999</v>
       </c>
       <c r="C323" s="3">
         <v>23</v>

</xml_diff>